<commit_message>
change algrothirm at export room function
</commit_message>
<xml_diff>
--- a/public/export/phòng nhạc.xlsx
+++ b/public/export/phòng nhạc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>THỜI KHÓA BIỂU PHÒNG phòng nhạc</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Trần Văn Thành-2C</t>
-  </si>
-  <si>
-    <t>Trần Văn Thành-2Đ</t>
   </si>
   <si>
     <t>Trần Văn Thành-1C</t>
@@ -535,7 +532,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" s="5"/>
     </row>
@@ -549,7 +546,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="5"/>
     </row>
@@ -561,13 +558,13 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -579,13 +576,13 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -597,7 +594,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -605,7 +602,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -635,10 +632,10 @@
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -652,7 +649,7 @@
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>

</xml_diff>

<commit_message>
sua lai phan xuat phan cong chuyen mon
</commit_message>
<xml_diff>
--- a/public/export/phòng nhạc.xlsx
+++ b/public/export/phòng nhạc.xlsx
@@ -48,49 +48,49 @@
     <t>Sáng</t>
   </si>
   <si>
-    <t>Âm nhạc-Trần Văn Thành-2B</t>
-  </si>
-  <si>
-    <t>Âm nhạc-Trần Văn Thành-2C</t>
-  </si>
-  <si>
-    <t>Âm nhạc-Trần Văn Thành-2Đ</t>
-  </si>
-  <si>
-    <t>Âm nhạc-Trần Văn Thành-1C</t>
-  </si>
-  <si>
-    <t>Âm nhạc-Trần Văn Thành-4A</t>
-  </si>
-  <si>
-    <t>Âm nhạc-Trần Văn Thành-2D</t>
-  </si>
-  <si>
-    <t>Âm nhạc-Trần Văn Thành-2A</t>
-  </si>
-  <si>
-    <t>Âm nhạc-Trần Văn Thành-4B</t>
-  </si>
-  <si>
-    <t>Âm nhạc-Trần Văn Thành-1D</t>
-  </si>
-  <si>
-    <t>Âm nhạc-Trần Văn Thành-5B</t>
-  </si>
-  <si>
-    <t>Âm nhạc-Trần Văn Thành-5A</t>
+    <t>Âm nhạc-Văn-Thành-2B</t>
+  </si>
+  <si>
+    <t>Âm nhạc-Văn-Thành-2C</t>
+  </si>
+  <si>
+    <t>Âm nhạc-Văn-Thành-2Đ</t>
+  </si>
+  <si>
+    <t>Âm nhạc-Văn-Thành-1C</t>
+  </si>
+  <si>
+    <t>Âm nhạc-Văn-Thành-4A</t>
+  </si>
+  <si>
+    <t>Âm nhạc-Văn-Thành-2D</t>
+  </si>
+  <si>
+    <t>Âm nhạc-Văn-Thành-2A</t>
+  </si>
+  <si>
+    <t>Âm nhạc-Văn-Thành-4B</t>
+  </si>
+  <si>
+    <t>Âm nhạc-Văn-Thành-1D</t>
+  </si>
+  <si>
+    <t>Âm nhạc-Văn-Thành-5B</t>
+  </si>
+  <si>
+    <t>Âm nhạc-Văn-Thành-5A</t>
   </si>
   <si>
     <t>Chiều</t>
   </si>
   <si>
-    <t>Âm nhạc-Trần Văn Thành-3A</t>
-  </si>
-  <si>
-    <t>Âm nhạc-Trần Văn Thành-3C</t>
-  </si>
-  <si>
-    <t>Âm nhạc-Trần Văn Thành-3B</t>
+    <t>Âm nhạc-Văn-Thành-3A</t>
+  </si>
+  <si>
+    <t>Âm nhạc-Văn-Thành-3C</t>
+  </si>
+  <si>
+    <t>Âm nhạc-Văn-Thành-3B</t>
   </si>
 </sst>
 </file>
@@ -477,11 +477,11 @@
   <cols>
     <col min="1" max="1" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="30.563965" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="30.563965" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="30.563965" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="30.563965" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="30.563965" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="6.998291" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>

</xml_diff>